<commit_message>
Fix for unicode characters
</commit_message>
<xml_diff>
--- a/videos/Website videos.xlsx
+++ b/videos/Website videos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="402">
   <si>
     <t>#</t>
   </si>
@@ -244,7 +244,7 @@
     <t>Georg Benda</t>
   </si>
   <si>
-    <t>Piano, Best of</t>
+    <t>Best of</t>
   </si>
   <si>
     <t>https://youtu.be/4oPnFsYPNX8</t>
@@ -328,9 +328,6 @@
     <t>We Wish You A Merry Christmas</t>
   </si>
   <si>
-    <t>Traditional</t>
-  </si>
-  <si>
     <t>Christmas, Best of,</t>
   </si>
   <si>
@@ -1057,15 +1054,12 @@
     <t>The Grand Entrance</t>
   </si>
   <si>
-    <t>Nannie's birthday</t>
+    <t>Nannie's birthday, Live,</t>
   </si>
   <si>
     <t>https://youtu.be/tBK2iplfs7w</t>
   </si>
   <si>
-    <t>Nannie's birthday, Live,</t>
-  </si>
-  <si>
     <t>https://youtu.be/i8f0oKvUsvM</t>
   </si>
   <si>
@@ -1190,6 +1184,39 @@
   </si>
   <si>
     <t>https://youtu.be/cB-A8gxaw98</t>
+  </si>
+  <si>
+    <t>Law Collection Trailer</t>
+  </si>
+  <si>
+    <t>https://youtu.be/68C1X1wEAZc</t>
+  </si>
+  <si>
+    <t>Hallelujah</t>
+  </si>
+  <si>
+    <t>Leonard Cohen</t>
+  </si>
+  <si>
+    <t>https://youtu.be/IfWMiGK0p8E</t>
+  </si>
+  <si>
+    <t>Tears in Heaven</t>
+  </si>
+  <si>
+    <t>Eric Clapton</t>
+  </si>
+  <si>
+    <t>https://youtu.be/MtB5VL1F4oE</t>
+  </si>
+  <si>
+    <t>With You</t>
+  </si>
+  <si>
+    <t>Brian Mazzaferri</t>
+  </si>
+  <si>
+    <t>https://youtu.be/4nzEnXQj2Fc</t>
   </si>
 </sst>
 </file>
@@ -2066,6 +2093,9 @@
         <v>2010.0</v>
       </c>
       <c r="F21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>77</v>
       </c>
       <c r="H21" s="2" t="s">
@@ -2073,7 +2103,7 @@
       </c>
       <c r="I21" s="3" t="str">
         <f>F21&amp;" performed by "&amp;(IF(D21="M","Matthew","Allie"))</f>
-        <v>Piano, Best of performed by Matthew</v>
+        <v>Piano performed by Matthew</v>
       </c>
     </row>
     <row r="22">
@@ -2308,9 +2338,6 @@
       <c r="B30" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="D30" s="1" t="s">
         <v>55</v>
       </c>
@@ -2321,13 +2348,13 @@
         <v>12</v>
       </c>
       <c r="G30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="I30" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="31">
@@ -2335,10 +2362,10 @@
         <v>30.0</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>11</v>
@@ -2350,7 +2377,7 @@
         <v>84</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I31" s="3" t="str">
         <f t="shared" ref="I31:I32" si="5">F31&amp;" performed by "&amp;(IF(D31="M","Matthew","Allie"))</f>
@@ -2362,10 +2389,10 @@
         <v>31.0</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>11</v>
@@ -2377,7 +2404,7 @@
         <v>12</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I32" s="3" t="str">
         <f t="shared" si="5"/>
@@ -2389,7 +2416,7 @@
         <v>32.0</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
@@ -2405,7 +2432,7 @@
         <v>57</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>82</v>
@@ -2416,7 +2443,7 @@
         <v>33.0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>23</v>
@@ -2431,7 +2458,7 @@
         <v>12</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I34" s="3" t="str">
         <f t="shared" ref="I34:I43" si="6">F34&amp;" performed by "&amp;(IF(D34="M","Matthew","Allie"))</f>
@@ -2443,10 +2470,10 @@
         <v>34.0</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>11</v>
@@ -2458,7 +2485,7 @@
         <v>84</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I35" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2470,10 +2497,10 @@
         <v>35.0</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>11</v>
@@ -2485,7 +2512,7 @@
         <v>12</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I36" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2497,10 +2524,10 @@
         <v>36.0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -2512,7 +2539,7 @@
         <v>12</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I37" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2524,10 +2551,10 @@
         <v>37.0</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>11</v>
@@ -2539,7 +2566,7 @@
         <v>12</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I38" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2551,10 +2578,10 @@
         <v>38.0</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
@@ -2566,7 +2593,7 @@
         <v>12</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I39" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2578,10 +2605,10 @@
         <v>39.0</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>11</v>
@@ -2593,10 +2620,10 @@
         <v>12</v>
       </c>
       <c r="G40" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H40" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="I40" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2608,10 +2635,10 @@
         <v>40.0</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>11</v>
@@ -2623,7 +2650,7 @@
         <v>12</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I41" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2635,10 +2662,10 @@
         <v>41.0</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>11</v>
@@ -2653,7 +2680,7 @@
         <v>88</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I42" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2665,10 +2692,10 @@
         <v>42.0</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>11</v>
@@ -2680,7 +2707,7 @@
         <v>84</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I43" s="3" t="str">
         <f t="shared" si="6"/>
@@ -2692,10 +2719,10 @@
         <v>43.0</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>11</v>
@@ -2707,7 +2734,7 @@
         <v>80</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>82</v>
@@ -2718,10 +2745,10 @@
         <v>44.0</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
@@ -2733,10 +2760,10 @@
         <v>12</v>
       </c>
       <c r="G45" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H45" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="I45" s="3" t="str">
         <f t="shared" ref="I45:I46" si="7">F45&amp;" performed by "&amp;(IF(D45="M","Matthew","Allie"))</f>
@@ -2748,10 +2775,10 @@
         <v>45.0</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
@@ -2763,10 +2790,10 @@
         <v>12</v>
       </c>
       <c r="G46" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H46" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>156</v>
       </c>
       <c r="I46" s="3" t="str">
         <f t="shared" si="7"/>
@@ -2778,7 +2805,7 @@
         <v>46.0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
@@ -2792,7 +2819,7 @@
         <v>57</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48">
@@ -2800,10 +2827,10 @@
         <v>47.0</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>11</v>
@@ -2818,7 +2845,7 @@
         <v>65</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I48" s="3" t="str">
         <f t="shared" ref="I48:I74" si="8">F48&amp;" performed by "&amp;(IF(D48="M","Matthew","Allie"))</f>
@@ -2830,10 +2857,10 @@
         <v>48.0</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>11</v>
@@ -2845,7 +2872,7 @@
         <v>12</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I49" s="3" t="str">
         <f t="shared" si="8"/>
@@ -2857,10 +2884,10 @@
         <v>49.0</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -2872,7 +2899,7 @@
         <v>12</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I50" s="3" t="str">
         <f t="shared" si="8"/>
@@ -2884,7 +2911,7 @@
         <v>50.0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>94</v>
@@ -2902,7 +2929,7 @@
         <v>102</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I51" s="3" t="str">
         <f t="shared" si="8"/>
@@ -2914,10 +2941,10 @@
         <v>51.0</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
@@ -2932,7 +2959,7 @@
         <v>13</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I52" s="3" t="str">
         <f t="shared" si="8"/>
@@ -2944,10 +2971,10 @@
         <v>52.0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -2959,10 +2986,10 @@
         <v>12</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I53" s="3" t="str">
         <f t="shared" si="8"/>
@@ -2974,10 +3001,10 @@
         <v>53.0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>11</v>
@@ -2989,10 +3016,10 @@
         <v>12</v>
       </c>
       <c r="G54" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="H54" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="I54" s="3" t="str">
         <f t="shared" si="8"/>
@@ -3004,10 +3031,10 @@
         <v>54.0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -3019,7 +3046,7 @@
         <v>12</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I55" s="3" t="str">
         <f t="shared" si="8"/>
@@ -3031,10 +3058,10 @@
         <v>55.0</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -3046,10 +3073,10 @@
         <v>12</v>
       </c>
       <c r="G56" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H56" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="I56" s="3" t="str">
         <f t="shared" si="8"/>
@@ -3061,10 +3088,10 @@
         <v>56.0</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -3076,7 +3103,7 @@
         <v>12</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I57" s="3" t="str">
         <f t="shared" si="8"/>
@@ -3088,10 +3115,10 @@
         <v>57.0</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>11</v>
@@ -3106,7 +3133,7 @@
         <v>102</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I58" s="3" t="str">
         <f t="shared" si="8"/>
@@ -3118,10 +3145,10 @@
         <v>58.0</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -3136,7 +3163,7 @@
         <v>52</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I59" s="3" t="str">
         <f t="shared" si="8"/>
@@ -3148,10 +3175,10 @@
         <v>59.0</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>194</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>11</v>
@@ -3166,7 +3193,7 @@
         <v>52</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I60" s="3" t="str">
         <f t="shared" si="8"/>
@@ -3178,10 +3205,10 @@
         <v>60.0</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
@@ -3196,7 +3223,7 @@
         <v>13</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I61" s="3" t="str">
         <f t="shared" si="8"/>
@@ -3208,10 +3235,10 @@
         <v>61.0</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>11</v>
@@ -3223,10 +3250,10 @@
         <v>12</v>
       </c>
       <c r="G62" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="H62" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="I62" s="3" t="str">
         <f t="shared" si="8"/>
@@ -3256,7 +3283,7 @@
         <v>19</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I63" s="3" t="str">
         <f t="shared" si="8"/>
@@ -3268,10 +3295,10 @@
         <v>63.0</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>11</v>
@@ -3283,7 +3310,7 @@
         <v>12</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I64" s="3" t="str">
         <f t="shared" si="8"/>
@@ -3295,10 +3322,10 @@
         <v>64.0</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -3313,7 +3340,7 @@
         <v>65</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I65" s="3" t="str">
         <f t="shared" si="8"/>
@@ -3325,10 +3352,10 @@
         <v>65.0</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -3343,7 +3370,7 @@
         <v>19</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I66" s="3" t="str">
         <f t="shared" si="8"/>
@@ -3355,10 +3382,10 @@
         <v>66.0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -3370,7 +3397,7 @@
         <v>12</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I67" s="3" t="str">
         <f t="shared" si="8"/>
@@ -3382,10 +3409,10 @@
         <v>67.0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -3397,10 +3424,10 @@
         <v>12</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I68" s="3" t="str">
         <f t="shared" si="8"/>
@@ -3412,10 +3439,10 @@
         <v>68.0</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>215</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -3427,7 +3454,7 @@
         <v>12</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I69" s="3" t="str">
         <f t="shared" si="8"/>
@@ -3439,10 +3466,10 @@
         <v>69.0</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
@@ -3454,7 +3481,7 @@
         <v>12</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I70" s="3" t="str">
         <f t="shared" si="8"/>
@@ -3466,10 +3493,10 @@
         <v>70.0</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>219</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
@@ -3484,7 +3511,7 @@
         <v>19</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I71" s="3" t="str">
         <f t="shared" si="8"/>
@@ -3496,10 +3523,10 @@
         <v>71.0</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>11</v>
@@ -3511,7 +3538,7 @@
         <v>12</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I72" s="3" t="str">
         <f t="shared" si="8"/>
@@ -3523,10 +3550,10 @@
         <v>72.0</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>11</v>
@@ -3535,13 +3562,13 @@
         <v>2014.0</v>
       </c>
       <c r="F73" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H73" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>227</v>
       </c>
       <c r="I73" s="3" t="str">
         <f t="shared" si="8"/>
@@ -3553,10 +3580,10 @@
         <v>73.0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
@@ -3568,10 +3595,10 @@
         <v>12</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I74" s="3" t="str">
         <f t="shared" si="8"/>
@@ -3583,7 +3610,7 @@
         <v>74.0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
@@ -3597,10 +3624,10 @@
         <v>57</v>
       </c>
       <c r="H75" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="I75" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="I75" s="1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="76">
@@ -3608,10 +3635,7 @@
         <v>75.0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>105</v>
+        <v>232</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
@@ -3626,7 +3650,7 @@
         <v>19</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I76" s="3" t="str">
         <f t="shared" ref="I76:I98" si="9">F76&amp;" performed by "&amp;(IF(D76="M","Matthew","Allie"))</f>
@@ -3638,10 +3662,10 @@
         <v>76.0</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>11</v>
@@ -3656,7 +3680,7 @@
         <v>19</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I77" s="3" t="str">
         <f t="shared" si="9"/>
@@ -3668,10 +3692,7 @@
         <v>77.0</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>105</v>
+        <v>237</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>11</v>
@@ -3686,7 +3707,7 @@
         <v>19</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I78" s="3" t="str">
         <f t="shared" si="9"/>
@@ -3698,10 +3719,10 @@
         <v>78.0</v>
       </c>
       <c r="B79" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>11</v>
@@ -3713,7 +3734,7 @@
         <v>12</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I79" s="3" t="str">
         <f t="shared" si="9"/>
@@ -3725,10 +3746,10 @@
         <v>79.0</v>
       </c>
       <c r="B80" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>244</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
@@ -3740,7 +3761,7 @@
         <v>12</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I80" s="3" t="str">
         <f t="shared" si="9"/>
@@ -3752,10 +3773,10 @@
         <v>80.0</v>
       </c>
       <c r="B81" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C81" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>247</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>11</v>
@@ -3770,7 +3791,7 @@
         <v>102</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I81" s="3" t="str">
         <f t="shared" si="9"/>
@@ -3782,10 +3803,10 @@
         <v>81.0</v>
       </c>
       <c r="B82" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C82" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>11</v>
@@ -3800,7 +3821,7 @@
         <v>65</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I82" s="3" t="str">
         <f t="shared" si="9"/>
@@ -3812,10 +3833,10 @@
         <v>82.0</v>
       </c>
       <c r="B83" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>11</v>
@@ -3827,10 +3848,10 @@
         <v>12</v>
       </c>
       <c r="G83" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="H83" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="H83" s="2" t="s">
-        <v>255</v>
       </c>
       <c r="I83" s="3" t="str">
         <f t="shared" si="9"/>
@@ -3842,10 +3863,10 @@
         <v>83.0</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>11</v>
@@ -3857,10 +3878,10 @@
         <v>12</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I84" s="3" t="str">
         <f t="shared" si="9"/>
@@ -3872,10 +3893,10 @@
         <v>84.0</v>
       </c>
       <c r="B85" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>259</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>11</v>
@@ -3887,7 +3908,7 @@
         <v>12</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I85" s="3" t="str">
         <f t="shared" si="9"/>
@@ -3899,10 +3920,10 @@
         <v>85.0</v>
       </c>
       <c r="B86" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>262</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>11</v>
@@ -3914,10 +3935,10 @@
         <v>12</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I86" s="3" t="str">
         <f t="shared" si="9"/>
@@ -3929,10 +3950,10 @@
         <v>86.0</v>
       </c>
       <c r="B87" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>11</v>
@@ -3944,7 +3965,7 @@
         <v>12</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I87" s="3" t="str">
         <f t="shared" si="9"/>
@@ -3956,10 +3977,10 @@
         <v>87.0</v>
       </c>
       <c r="B88" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>11</v>
@@ -3971,10 +3992,10 @@
         <v>12</v>
       </c>
       <c r="G88" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="H88" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="H88" s="2" t="s">
-        <v>268</v>
       </c>
       <c r="I88" s="3" t="str">
         <f t="shared" si="9"/>
@@ -3986,10 +4007,10 @@
         <v>88.0</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>11</v>
@@ -4001,10 +4022,10 @@
         <v>12</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I89" s="3" t="str">
         <f t="shared" si="9"/>
@@ -4016,10 +4037,10 @@
         <v>89.0</v>
       </c>
       <c r="B90" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C90" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>272</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>11</v>
@@ -4031,10 +4052,10 @@
         <v>12</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I90" s="3" t="str">
         <f t="shared" si="9"/>
@@ -4046,10 +4067,10 @@
         <v>90.0</v>
       </c>
       <c r="B91" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>275</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>11</v>
@@ -4064,7 +4085,7 @@
         <v>65</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I91" s="3" t="str">
         <f t="shared" si="9"/>
@@ -4076,10 +4097,10 @@
         <v>91.0</v>
       </c>
       <c r="B92" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C92" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>278</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>11</v>
@@ -4091,7 +4112,7 @@
         <v>12</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I92" s="3" t="str">
         <f t="shared" si="9"/>
@@ -4103,10 +4124,10 @@
         <v>92.0</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>11</v>
@@ -4115,13 +4136,13 @@
         <v>2015.0</v>
       </c>
       <c r="F93" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H93" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="H93" s="2" t="s">
-        <v>282</v>
       </c>
       <c r="I93" s="3" t="str">
         <f t="shared" si="9"/>
@@ -4133,10 +4154,10 @@
         <v>93.0</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>11</v>
@@ -4145,13 +4166,13 @@
         <v>2015.0</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>65</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I94" s="3" t="str">
         <f t="shared" si="9"/>
@@ -4163,10 +4184,10 @@
         <v>94.0</v>
       </c>
       <c r="B95" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>286</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>11</v>
@@ -4178,10 +4199,10 @@
         <v>12</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I95" s="3" t="str">
         <f t="shared" si="9"/>
@@ -4193,10 +4214,10 @@
         <v>95.0</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>11</v>
@@ -4208,10 +4229,10 @@
         <v>12</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I96" s="3" t="str">
         <f t="shared" si="9"/>
@@ -4223,7 +4244,7 @@
         <v>96.0</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>94</v>
@@ -4241,7 +4262,7 @@
         <v>13</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I97" s="3" t="str">
         <f t="shared" si="9"/>
@@ -4253,10 +4274,10 @@
         <v>97.0</v>
       </c>
       <c r="B98" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C98" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>11</v>
@@ -4268,10 +4289,10 @@
         <v>12</v>
       </c>
       <c r="G98" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="H98" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="H98" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="I98" s="3" t="str">
         <f t="shared" si="9"/>
@@ -4283,10 +4304,10 @@
         <v>98.0</v>
       </c>
       <c r="B99" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C99" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>297</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>55</v>
@@ -4295,16 +4316,16 @@
         <v>2016.0</v>
       </c>
       <c r="F99" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H99" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="G99" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="H99" s="2" t="s">
+      <c r="I99" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="I99" s="1" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="100">
@@ -4312,10 +4333,10 @@
         <v>99.0</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>55</v>
@@ -4324,16 +4345,16 @@
         <v>2016.0</v>
       </c>
       <c r="F100" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H100" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="G100" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="H100" s="2" t="s">
+      <c r="I100" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="I100" s="1" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="101">
@@ -4341,7 +4362,7 @@
         <v>100.0</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>94</v>
@@ -4359,7 +4380,7 @@
         <v>13</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I101" s="3" t="str">
         <f t="shared" ref="I101:I105" si="10">F101&amp;" performed by "&amp;(IF(D101="M","Matthew","Allie"))</f>
@@ -4371,10 +4392,10 @@
         <v>101.0</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>11</v>
@@ -4386,10 +4407,10 @@
         <v>12</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I102" s="3" t="str">
         <f t="shared" si="10"/>
@@ -4401,10 +4422,10 @@
         <v>102.0</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>11</v>
@@ -4416,10 +4437,10 @@
         <v>12</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I103" s="3" t="str">
         <f t="shared" si="10"/>
@@ -4431,10 +4452,10 @@
         <v>103.0</v>
       </c>
       <c r="B104" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>311</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>312</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>11</v>
@@ -4446,10 +4467,10 @@
         <v>12</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I104" s="3" t="str">
         <f t="shared" si="10"/>
@@ -4461,10 +4482,10 @@
         <v>104.0</v>
       </c>
       <c r="B105" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>315</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>11</v>
@@ -4476,10 +4497,10 @@
         <v>12</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I105" s="3" t="str">
         <f t="shared" si="10"/>
@@ -4491,7 +4512,7 @@
         <v>105.0</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C106" s="1"/>
       <c r="D106" s="1" t="s">
@@ -4501,16 +4522,16 @@
         <v>2017.0</v>
       </c>
       <c r="F106" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H106" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="G106" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="H106" s="2" t="s">
+      <c r="I106" s="1" t="s">
         <v>319</v>
-      </c>
-      <c r="I106" s="1" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="107">
@@ -4518,10 +4539,10 @@
         <v>106.0</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>11</v>
@@ -4536,7 +4557,7 @@
         <v>13</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I107" s="3" t="str">
         <f>F107&amp;" performed by "&amp;(IF(D107="M","Matthew","Allie"))</f>
@@ -4548,10 +4569,10 @@
         <v>107.0</v>
       </c>
       <c r="B108" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>323</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>324</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>55</v>
@@ -4560,16 +4581,16 @@
         <v>2017.0</v>
       </c>
       <c r="F108" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H108" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="G108" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="H108" s="2" t="s">
+      <c r="I108" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="I108" s="1" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="109">
@@ -4577,10 +4598,10 @@
         <v>108.0</v>
       </c>
       <c r="B109" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C109" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>329</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>11</v>
@@ -4592,10 +4613,10 @@
         <v>12</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I109" s="3" t="str">
         <f t="shared" ref="I109:I110" si="11">F109&amp;" performed by "&amp;(IF(D109="M","Matthew","Allie"))</f>
@@ -4607,10 +4628,10 @@
         <v>109.0</v>
       </c>
       <c r="B110" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C110" s="1" t="s">
         <v>331</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>332</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>11</v>
@@ -4625,7 +4646,7 @@
         <v>13</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I110" s="3" t="str">
         <f t="shared" si="11"/>
@@ -4637,7 +4658,7 @@
         <v>110.0</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>55</v>
@@ -4649,10 +4670,10 @@
         <v>57</v>
       </c>
       <c r="H111" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="I111" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="I111" s="1" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="112">
@@ -4660,10 +4681,10 @@
         <v>111.0</v>
       </c>
       <c r="B112" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D112" s="1" t="s">
         <v>337</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>338</v>
       </c>
       <c r="E112" s="1">
         <v>2013.0</v>
@@ -4672,10 +4693,10 @@
         <v>57</v>
       </c>
       <c r="H112" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="I112" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="I112" s="1" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="113">
@@ -4683,10 +4704,10 @@
         <v>112.0</v>
       </c>
       <c r="B113" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>341</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>342</v>
       </c>
       <c r="E113" s="1">
         <v>2012.0</v>
@@ -4695,10 +4716,10 @@
         <v>57</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="114">
@@ -4706,16 +4727,19 @@
         <v>113.0</v>
       </c>
       <c r="B114" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="D114" s="1" t="s">
         <v>344</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>345</v>
       </c>
       <c r="E114" s="1">
         <v>2004.0</v>
       </c>
+      <c r="G114" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="H114" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="115">
@@ -4723,16 +4747,16 @@
         <v>114.0</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E115" s="1">
         <v>2014.0</v>
       </c>
       <c r="G115" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="H115" s="2" t="s">
         <v>348</v>
-      </c>
-      <c r="H115" s="2" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="116">
@@ -4740,10 +4764,10 @@
         <v>115.0</v>
       </c>
       <c r="B116" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>11</v>
@@ -4755,13 +4779,13 @@
         <v>12</v>
       </c>
       <c r="G116" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="H116" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="I116" s="3" t="s">
         <v>350</v>
-      </c>
-      <c r="H116" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="I116" s="3" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="117">
@@ -4769,28 +4793,28 @@
         <v>116.0</v>
       </c>
       <c r="B117" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D117" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>355</v>
       </c>
       <c r="E117" s="1">
         <v>2014.0</v>
       </c>
       <c r="F117" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="H117" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="I117" s="1" t="s">
         <v>356</v>
-      </c>
-      <c r="G117" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="H117" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="I117" s="1" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="118">
@@ -4798,10 +4822,10 @@
         <v>117.0</v>
       </c>
       <c r="B118" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C118" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>11</v>
@@ -4813,13 +4837,13 @@
         <v>12</v>
       </c>
       <c r="G118" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="H118" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="I118" s="3" t="s">
         <v>350</v>
-      </c>
-      <c r="H118" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="I118" s="3" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="119">
@@ -4827,25 +4851,25 @@
         <v>118.0</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E119" s="1">
         <v>2014.0</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="H119" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="120">
@@ -4853,10 +4877,10 @@
         <v>119.0</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>11</v>
@@ -4868,10 +4892,10 @@
         <v>12</v>
       </c>
       <c r="H120" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="I120" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="121">
@@ -4879,10 +4903,10 @@
         <v>120.0</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>11</v>
@@ -4894,10 +4918,10 @@
         <v>12</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="I121" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="122">
@@ -4905,10 +4929,10 @@
         <v>121.0</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>11</v>
@@ -4920,13 +4944,13 @@
         <v>12</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="I122" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="123">
@@ -4934,10 +4958,10 @@
         <v>122.0</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>11</v>
@@ -4949,13 +4973,13 @@
         <v>12</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="I123" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="124">
@@ -4963,10 +4987,10 @@
         <v>123.0</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>11</v>
@@ -4981,10 +5005,10 @@
         <v>13</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="I124" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="125">
@@ -4992,10 +5016,10 @@
         <v>124.0</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>11</v>
@@ -5007,10 +5031,10 @@
         <v>12</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="I125" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="126">
@@ -5018,10 +5042,10 @@
         <v>125.0</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>11</v>
@@ -5033,13 +5057,13 @@
         <v>12</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I126" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="127">
@@ -5047,10 +5071,10 @@
         <v>126.0</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>11</v>
@@ -5062,13 +5086,13 @@
         <v>12</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I127" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="128">
@@ -5076,10 +5100,10 @@
         <v>127.0</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>11</v>
@@ -5091,13 +5115,13 @@
         <v>12</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H128" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="I128" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="129">
@@ -5105,10 +5129,10 @@
         <v>128.0</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>11</v>
@@ -5120,13 +5144,13 @@
         <v>12</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H129" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="I129" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="130">
@@ -5134,10 +5158,10 @@
         <v>129.0</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>11</v>
@@ -5149,33 +5173,120 @@
         <v>12</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H130" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I130" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1">
         <v>130.0</v>
       </c>
+      <c r="B131" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E131" s="1">
+        <v>2019.0</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="H131" s="2" t="s">
+        <v>392</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1">
         <v>131.0</v>
       </c>
+      <c r="B132" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E132" s="1">
+        <v>2019.0</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="G132" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H132" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="I132" s="1" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1">
         <v>132.0</v>
       </c>
+      <c r="B133" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E133" s="1">
+        <v>2019.0</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H133" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="I133" s="1" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1">
         <v>133.0</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E134" s="1">
+        <v>2019.0</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H134" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="I134" s="1" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="135">
@@ -5314,7 +5425,11 @@
     <hyperlink r:id="rId127" ref="H128"/>
     <hyperlink r:id="rId128" ref="H129"/>
     <hyperlink r:id="rId129" ref="H130"/>
+    <hyperlink r:id="rId130" ref="H131"/>
+    <hyperlink r:id="rId131" ref="H132"/>
+    <hyperlink r:id="rId132" ref="H133"/>
+    <hyperlink r:id="rId133" ref="H134"/>
   </hyperlinks>
-  <drawing r:id="rId130"/>
+  <drawing r:id="rId134"/>
 </worksheet>
 </file>
</xml_diff>